<commit_message>
Updated TDD format to xlsx
</commit_message>
<xml_diff>
--- a/Report Examples/Leave/PR16_ZLVEABT_ Absence_Tracker_by_date_ UBA_NIGERIA.xlsx
+++ b/Report Examples/Leave/PR16_ZLVEABT_ Absence_Tracker_by_date_ UBA_NIGERIA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adebukola.imoyo\Documents\My Documents\HR Application Implementation Project\Documents from SAGE\August Workshops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ParityLoan1\Desktop\Sage\Leave\TDD\Updated_TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Absence Tracker" sheetId="1" r:id="rId1"/>
@@ -249,23 +249,11 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -276,6 +264,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,130 +570,142 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="6" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="7"/>
+      <c r="V3" s="12"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
     </row>
     <row r="5" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="V2:V3"/>
@@ -703,18 +715,6 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>